<commit_message>
created generateEmail.js to create eml files and edited addressBook.js and invoiceFunction.js for needed functionalities
</commit_message>
<xml_diff>
--- a/resources/unitList.xlsx
+++ b/resources/unitList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristianguarino/projects/invoice_generator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C86D171-143C-604F-AB2D-78AEBAA26DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D13E31-EFBD-AE41-8D85-A74E992C601D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-49100" yWindow="2760" windowWidth="17620" windowHeight="17440" xr2:uid="{62FF9A3F-09B1-4E41-A48B-AC3A7439D0C5}"/>
+    <workbookView xWindow="32800" yWindow="2200" windowWidth="17620" windowHeight="17440" xr2:uid="{62FF9A3F-09B1-4E41-A48B-AC3A7439D0C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
     <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>